<commit_message>
Queue size for K8s
</commit_message>
<xml_diff>
--- a/Data/AllResults_Aluminium Hydroxide-0.291Gm + Magnesium Hydroxide-98Mg + Oxetacaine-10Mg.xlsx
+++ b/Data/AllResults_Aluminium Hydroxide-0.291Gm + Magnesium Hydroxide-98Mg + Oxetacaine-10Mg.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="90">
   <si>
     <t>Molecule</t>
   </si>
@@ -567,19 +567,19 @@
         <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C8" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="D8" t="s">
         <v>3</v>
       </c>
       <c r="E8" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="F8" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="G8" t="s">
         <v>15</v>
@@ -599,19 +599,19 @@
         <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C9" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D9" t="s">
         <v>3</v>
       </c>
       <c r="E9" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="F9" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="G9" t="s">
         <v>15</v>
@@ -631,7 +631,7 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C10" t="s">
         <v>39</v>
@@ -640,7 +640,7 @@
         <v>3</v>
       </c>
       <c r="E10" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="F10" t="s">
         <v>14</v>
@@ -983,28 +983,28 @@
         <v>10</v>
       </c>
       <c r="B21" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="C21" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="D21" t="s">
         <v>3</v>
       </c>
       <c r="E21" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="F21" t="s">
-        <v>22</v>
+        <v>87</v>
       </c>
       <c r="G21" t="s">
         <v>15</v>
       </c>
       <c r="H21" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="I21" t="s">
-        <v>17</v>
+        <v>89</v>
       </c>
       <c r="J21" t="s">
         <v>18</v>
@@ -1015,28 +1015,28 @@
         <v>10</v>
       </c>
       <c r="B22" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C22" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="D22" t="s">
         <v>3</v>
       </c>
       <c r="E22" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="F22" t="s">
-        <v>87</v>
+        <v>22</v>
       </c>
       <c r="G22" t="s">
         <v>15</v>
       </c>
       <c r="H22" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="I22" t="s">
-        <v>89</v>
+        <v>17</v>
       </c>
       <c r="J22" t="s">
         <v>18</v>

</xml_diff>